<commit_message>
Change pin layout for WT32-SC01
</commit_message>
<xml_diff>
--- a/Hardware/Brochage ESP32.xlsx
+++ b/Hardware/Brochage ESP32.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alixa\github\Xila Embedded\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00426350-9CCE-49AB-9E38-F1DF5EB306E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD030A84-B535-4075-9D04-935EAE17C230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="239">
   <si>
     <t>ADC</t>
   </si>
@@ -703,15 +703,9 @@
     <t>W32-SC01</t>
   </si>
   <si>
-    <t>LCD</t>
-  </si>
-  <si>
     <t>USED</t>
   </si>
   <si>
-    <t>Touch</t>
-  </si>
-  <si>
     <t>SD CLK</t>
   </si>
   <si>
@@ -722,13 +716,43 @@
   </si>
   <si>
     <t>SD CS</t>
+  </si>
+  <si>
+    <t>LCD CLK</t>
+  </si>
+  <si>
+    <t>LCD MOSI</t>
+  </si>
+  <si>
+    <t>LCD MISO</t>
+  </si>
+  <si>
+    <t>LCD DC</t>
+  </si>
+  <si>
+    <t>LCD CS</t>
+  </si>
+  <si>
+    <t>LCD RST</t>
+  </si>
+  <si>
+    <t>TOUCH SDA</t>
+  </si>
+  <si>
+    <t>TOUCH SCL</t>
+  </si>
+  <si>
+    <t>BACKLIGHT PWM</t>
+  </si>
+  <si>
+    <t>NON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,8 +795,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,6 +864,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -871,10 +907,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -942,13 +979,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1266,7 +1312,7 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1331,7 @@
     <col min="16" max="16" width="14.140625" style="2" customWidth="1"/>
     <col min="17" max="17" width="43.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="34" style="2" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" style="25" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" style="26" customWidth="1"/>
     <col min="20" max="20" width="24.5703125" style="2" customWidth="1"/>
     <col min="21" max="21" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1346,7 +1392,7 @@
       </c>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="25" t="s">
         <v>223</v>
       </c>
     </row>
@@ -1387,7 +1433,6 @@
         <v>72</v>
       </c>
       <c r="R2" s="20"/>
-      <c r="S2" s="24"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1469,8 +1514,8 @@
       <c r="R4" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="S4" s="24" t="s">
-        <v>230</v>
+      <c r="S4" s="27" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1553,7 +1598,9 @@
       <c r="R6" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="S6" s="24"/>
+      <c r="S6" s="27" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1590,7 +1637,7 @@
       <c r="R7" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="27" t="s">
         <v>227</v>
       </c>
     </row>
@@ -1633,7 +1680,6 @@
       <c r="R8" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="S8" s="24"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -1674,7 +1720,6 @@
       <c r="R9" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="S9" s="24"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -1883,7 +1928,9 @@
       <c r="R14" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="S14" s="24"/>
+      <c r="S14" s="24" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1931,7 +1978,7 @@
         <v>214</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1980,7 +2027,7 @@
         <v>214</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -2029,7 +2076,7 @@
         <v>214</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -2068,7 +2115,7 @@
         <v>215</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -2106,8 +2153,8 @@
       <c r="R19" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="S19" s="24" t="s">
-        <v>229</v>
+      <c r="S19" s="26" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -2143,8 +2190,8 @@
       <c r="R20" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="S20" s="24" t="s">
-        <v>226</v>
+      <c r="S20" s="27" t="s">
+        <v>235</v>
       </c>
       <c r="T20" s="4"/>
     </row>
@@ -2183,8 +2230,8 @@
       <c r="R21" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="S21" s="24" t="s">
-        <v>226</v>
+      <c r="S21" s="27" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -2221,7 +2268,7 @@
         <v>210</v>
       </c>
       <c r="S22" s="24" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -2260,7 +2307,7 @@
         <v>218</v>
       </c>
       <c r="S23" s="24" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2296,8 +2343,8 @@
       <c r="R24" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="S24" s="24" t="s">
-        <v>224</v>
+      <c r="S24" s="27" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -2415,7 +2462,9 @@
       <c r="R27" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="S27" s="24"/>
+      <c r="S27" s="28" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
@@ -2597,7 +2646,7 @@
         <v>213</v>
       </c>
       <c r="S32" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2636,7 +2685,7 @@
       </c>
       <c r="R33" s="8"/>
       <c r="S33" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>